<commit_message>
Fix version for publication 191ce959cc81cfe12b97e36dfaff5daf7a90b908
</commit_message>
<xml_diff>
--- a/release/prepare-publication-1.1.0/ig/StructureDefinition-BundleAgregateur.xlsx
+++ b/release/prepare-publication-1.1.0/ig/StructureDefinition-BundleAgregateur.xlsx
@@ -30,7 +30,7 @@
     <t>Version</t>
   </si>
   <si>
-    <t>1.1.0-trial-use</t>
+    <t>1.0.0</t>
   </si>
   <si>
     <t>Name</t>
@@ -45,7 +45,7 @@
     <t>Status</t>
   </si>
   <si>
-    <t>draft</t>
+    <t>active</t>
   </si>
   <si>
     <t>Experimental</t>
@@ -54,7 +54,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2024-09-04T16:00:39+00:00</t>
+    <t>2024-09-05T10:11:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>

</xml_diff>